<commit_message>
working on C# Heightmap to c++
</commit_message>
<xml_diff>
--- a/docs/vegetation.xlsx
+++ b/docs/vegetation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rico\Documents\CLionProjects\Valhalla\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868C40D5-8AD6-45C6-B1E6-E19DB6DAA805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0203C97-B385-476B-AF3F-7353A976F1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="1320" windowWidth="15660" windowHeight="10815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8160" yWindow="1665" windowWidth="15660" windowHeight="10815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vegetation" sheetId="1" r:id="rId1"/>
@@ -688,7 +688,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -868,6 +868,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1029,8 +1035,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1388,20 +1395,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y100" sqref="Y100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" customWidth="1"/>
+    <col min="26" max="26" width="18" customWidth="1"/>
     <col min="27" max="27" width="13.28515625" customWidth="1"/>
     <col min="28" max="28" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1505,7 +1514,7 @@
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>873</v>
       </c>
       <c r="B2">
@@ -1609,7 +1618,7 @@
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B3">
@@ -1713,7 +1722,7 @@
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B4">
@@ -1817,7 +1826,7 @@
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B5">
@@ -1921,7 +1930,7 @@
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B6">
@@ -2025,7 +2034,7 @@
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B7">
@@ -2129,7 +2138,7 @@
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B8">
@@ -2233,7 +2242,7 @@
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B9">
@@ -2337,7 +2346,7 @@
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B10">
@@ -2441,7 +2450,7 @@
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11">
@@ -2545,7 +2554,7 @@
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B12">
@@ -2649,7 +2658,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B13">
@@ -2753,7 +2762,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B14">
@@ -2857,7 +2866,7 @@
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>5</v>
       </c>
       <c r="B15">
@@ -2961,7 +2970,7 @@
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B16">
@@ -3065,7 +3074,7 @@
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>5</v>
       </c>
       <c r="B17">
@@ -3169,7 +3178,7 @@
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B18">
@@ -3273,7 +3282,7 @@
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B19">
@@ -3377,7 +3386,7 @@
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B20">
@@ -3481,7 +3490,7 @@
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B21">
@@ -3585,7 +3594,7 @@
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B22">
@@ -3689,7 +3698,7 @@
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B23">
@@ -3793,7 +3802,7 @@
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B24">
@@ -3897,7 +3906,7 @@
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B25">
@@ -4001,7 +4010,7 @@
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B26">
@@ -4105,7 +4114,7 @@
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>384</v>
       </c>
       <c r="B27">
@@ -4209,7 +4218,7 @@
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>128</v>
       </c>
       <c r="B28">
@@ -4313,7 +4322,7 @@
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B29">
@@ -4417,7 +4426,7 @@
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B30">
@@ -4521,7 +4530,7 @@
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B31">
@@ -4625,7 +4634,7 @@
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B32">
@@ -4729,7 +4738,7 @@
       </c>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B33">
@@ -4833,7 +4842,7 @@
       </c>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B34">
@@ -4937,7 +4946,7 @@
       </c>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B35">
@@ -5041,7 +5050,7 @@
       </c>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B36" t="s">
@@ -5145,7 +5154,7 @@
       </c>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B37">
@@ -5249,7 +5258,7 @@
       </c>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B38">
@@ -5353,7 +5362,7 @@
       </c>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B39">
@@ -5457,7 +5466,7 @@
       </c>
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B40">
@@ -5561,7 +5570,7 @@
       </c>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B41">
@@ -5665,7 +5674,7 @@
       </c>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B42">
@@ -5769,7 +5778,7 @@
       </c>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B43">
@@ -5873,7 +5882,7 @@
       </c>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B44">
@@ -5977,7 +5986,7 @@
       </c>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B45">
@@ -6081,7 +6090,7 @@
       </c>
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B46">
@@ -6185,7 +6194,7 @@
       </c>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B47">
@@ -6289,7 +6298,7 @@
       </c>
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B48">
@@ -6393,7 +6402,7 @@
       </c>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B49">
@@ -6497,7 +6506,7 @@
       </c>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B50">
@@ -6601,7 +6610,7 @@
       </c>
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B51">
@@ -6705,7 +6714,7 @@
       </c>
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B52">
@@ -6809,7 +6818,7 @@
       </c>
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B53">
@@ -6913,7 +6922,7 @@
       </c>
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B54">
@@ -7017,7 +7026,7 @@
       </c>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B55">
@@ -7121,7 +7130,7 @@
       </c>
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B56">
@@ -7225,7 +7234,7 @@
       </c>
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
@@ -7329,7 +7338,7 @@
       </c>
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B58">
@@ -7433,7 +7442,7 @@
       </c>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B59">
@@ -7537,7 +7546,7 @@
       </c>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B60">
@@ -7641,7 +7650,7 @@
       </c>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B61">
@@ -7745,7 +7754,7 @@
       </c>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B62">
@@ -7849,7 +7858,7 @@
       </c>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B63">
@@ -7953,7 +7962,7 @@
       </c>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B64">
@@ -8057,7 +8066,7 @@
       </c>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B65">
@@ -8161,7 +8170,7 @@
       </c>
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B66">
@@ -8265,7 +8274,7 @@
       </c>
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B67">
@@ -8369,7 +8378,7 @@
       </c>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B68">
@@ -8473,7 +8482,7 @@
       </c>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B69">
@@ -8577,7 +8586,7 @@
       </c>
     </row>
     <row r="70" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B70">
@@ -8681,7 +8690,7 @@
       </c>
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A71">
+      <c r="A71" s="1">
         <v>10</v>
       </c>
       <c r="B71" t="s">
@@ -8785,7 +8794,7 @@
       </c>
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B72">
@@ -8889,7 +8898,7 @@
       </c>
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B73" t="s">
@@ -8993,7 +9002,7 @@
       </c>
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B74">
@@ -9097,7 +9106,7 @@
       </c>
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A75">
+      <c r="A75" s="1">
         <v>11</v>
       </c>
       <c r="B75">
@@ -9201,7 +9210,7 @@
       </c>
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B76">
@@ -9305,7 +9314,7 @@
       </c>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B77">
@@ -9409,7 +9418,7 @@
       </c>
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A78">
+      <c r="A78" s="1">
         <v>17</v>
       </c>
       <c r="B78">
@@ -9513,7 +9522,7 @@
       </c>
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B79">
@@ -9617,7 +9626,7 @@
       </c>
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B80">
@@ -9721,7 +9730,7 @@
       </c>
     </row>
     <row r="81" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A81">
+      <c r="A81" s="1">
         <v>11</v>
       </c>
       <c r="B81">
@@ -9825,7 +9834,7 @@
       </c>
     </row>
     <row r="82" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B82">
@@ -9929,7 +9938,7 @@
       </c>
     </row>
     <row r="83" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B83">
@@ -10033,7 +10042,7 @@
       </c>
     </row>
     <row r="84" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B84">
@@ -10137,7 +10146,7 @@
       </c>
     </row>
     <row r="85" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="A85" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B85">
@@ -10241,7 +10250,7 @@
       </c>
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A86">
+      <c r="A86" s="1">
         <v>27</v>
       </c>
       <c r="B86">
@@ -10345,7 +10354,7 @@
       </c>
     </row>
     <row r="87" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A87">
+      <c r="A87" s="1">
         <v>3</v>
       </c>
       <c r="B87">
@@ -10449,7 +10458,7 @@
       </c>
     </row>
     <row r="88" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B88">
@@ -10553,7 +10562,7 @@
       </c>
     </row>
     <row r="89" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B89">
@@ -10657,7 +10666,7 @@
       </c>
     </row>
     <row r="90" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B90">
@@ -10761,7 +10770,7 @@
       </c>
     </row>
     <row r="91" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B91">
@@ -10865,7 +10874,7 @@
       </c>
     </row>
     <row r="92" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B92">
@@ -10969,7 +10978,7 @@
       </c>
     </row>
     <row r="93" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B93">
@@ -11073,7 +11082,7 @@
       </c>
     </row>
     <row r="94" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B94" t="s">
@@ -11177,7 +11186,7 @@
       </c>
     </row>
     <row r="95" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B95" t="s">
@@ -11281,7 +11290,7 @@
       </c>
     </row>
     <row r="96" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B96" t="s">
@@ -11385,7 +11394,7 @@
       </c>
     </row>
     <row r="97" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B97" t="s">
@@ -11489,7 +11498,7 @@
       </c>
     </row>
     <row r="98" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B98" t="s">
@@ -11593,7 +11602,7 @@
       </c>
     </row>
     <row r="99" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B99" t="s">
@@ -11697,7 +11706,7 @@
       </c>
     </row>
     <row r="100" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B100" t="s">
@@ -11801,7 +11810,7 @@
       </c>
     </row>
     <row r="101" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B101" t="s">
@@ -11905,7 +11914,7 @@
       </c>
     </row>
     <row r="102" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B102" t="s">
@@ -12009,7 +12018,7 @@
       </c>
     </row>
     <row r="103" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B103" t="s">
@@ -12113,7 +12122,7 @@
       </c>
     </row>
     <row r="104" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="A104" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B104" t="s">
@@ -12217,7 +12226,7 @@
       </c>
     </row>
     <row r="105" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A105" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B105" t="s">
@@ -12321,7 +12330,7 @@
       </c>
     </row>
     <row r="106" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="A106" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B106" t="s">
@@ -12425,7 +12434,7 @@
       </c>
     </row>
     <row r="107" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B107" t="s">
@@ -12529,7 +12538,7 @@
       </c>
     </row>
     <row r="108" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B108" t="s">
@@ -12633,7 +12642,7 @@
       </c>
     </row>
     <row r="109" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B109" t="s">
@@ -12737,7 +12746,7 @@
       </c>
     </row>
     <row r="110" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B110" t="s">
@@ -12841,7 +12850,7 @@
       </c>
     </row>
     <row r="111" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B111" t="s">
@@ -12945,7 +12954,7 @@
       </c>
     </row>
     <row r="112" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="A112" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B112" t="s">
@@ -13049,7 +13058,7 @@
       </c>
     </row>
     <row r="113" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B113" t="s">
@@ -13153,7 +13162,7 @@
       </c>
     </row>
     <row r="114" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B114" t="s">
@@ -13257,7 +13266,7 @@
       </c>
     </row>
     <row r="115" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B115" t="s">
@@ -13361,7 +13370,7 @@
       </c>
     </row>
     <row r="116" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B116" t="s">
@@ -13465,7 +13474,7 @@
       </c>
     </row>
     <row r="117" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B117" t="s">
@@ -13569,7 +13578,7 @@
       </c>
     </row>
     <row r="118" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B118" t="s">
@@ -13673,7 +13682,7 @@
       </c>
     </row>
     <row r="119" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B119" t="s">
@@ -13777,7 +13786,7 @@
       </c>
     </row>
     <row r="120" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B120" t="s">
@@ -13881,7 +13890,7 @@
       </c>
     </row>
     <row r="121" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="A121" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B121" t="s">
@@ -13985,7 +13994,7 @@
       </c>
     </row>
     <row r="122" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B122" t="s">
@@ -14089,7 +14098,7 @@
       </c>
     </row>
     <row r="123" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B123" t="s">
@@ -14194,5 +14203,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>